<commit_message>
finished draw_piechart() with embedded format function, generalized start row/col variables to pass in to function, removed appending totals to ws as draw_piechart() does that.
GPT: https://chatgpt.com/share/c645a871-80ab-4ffb-82a3-702a17821d5a
</commit_message>
<xml_diff>
--- a/Expense_Summary.xlsx
+++ b/Expense_Summary.xlsx
@@ -135,6 +135,1098 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>SEP23 Total Expenditure by Category</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'SEP23'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'SEP23'!$D$2:$D$9</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'SEP23'!$E$2:$E$9</f>
+            </numRef>
+          </val>
+        </ser>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>JUN24 Total Expenditure by Category</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'JUN24'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'JUN24'!$D$2:$D$9</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'JUN24'!$E$2:$E$9</f>
+            </numRef>
+          </val>
+        </ser>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>JUL24 Total Expenditure by Category</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'JUL24'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'JUL24'!$D$2:$D$9</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'JUL24'!$E$2:$E$9</f>
+            </numRef>
+          </val>
+        </ser>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>AUG24 Total Expenditure by Category</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'AUG24'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'AUG24'!$D$2:$D$8</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'AUG24'!$E$2:$E$8</f>
+            </numRef>
+          </val>
+        </ser>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>TEMPLATE Total Expenditure by Category</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'TEMPLATE'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'TEMPLATE'!$D$2:$D$1</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'TEMPLATE'!$F$1:$E$1</f>
+            </numRef>
+          </val>
+        </ser>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>OCT23 Total Expenditure by Category</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'OCT23'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'OCT23'!$D$2:$D$8</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'OCT23'!$E$2:$E$8</f>
+            </numRef>
+          </val>
+        </ser>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>NOV23 Total Expenditure by Category</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'NOV23'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'NOV23'!$D$2:$D$8</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'NOV23'!$E$2:$E$8</f>
+            </numRef>
+          </val>
+        </ser>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>DEC23 Total Expenditure by Category</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'DEC23'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'DEC23'!$D$2:$D$1</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'DEC23'!$F$1:$E$1</f>
+            </numRef>
+          </val>
+        </ser>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>JAN24 Total Expenditure by Category</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'JAN24'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'JAN24'!$D$2:$D$9</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'JAN24'!$E$2:$E$9</f>
+            </numRef>
+          </val>
+        </ser>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>FEB24 Total Expenditure by Category</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'FEB24'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'FEB24'!$D$2:$D$9</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'FEB24'!$E$2:$E$9</f>
+            </numRef>
+          </val>
+        </ser>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>MAR24 Total Expenditure by Category</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'MAR24'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'MAR24'!$D$2:$D$9</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'MAR24'!$E$2:$E$9</f>
+            </numRef>
+          </val>
+        </ser>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>APR24 Total Expenditure by Category</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'APR24'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'APR24'!$D$2:$D$9</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'APR24'!$E$2:$E$9</f>
+            </numRef>
+          </val>
+        </ser>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>MAY24 Total Expenditure by Category</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'MAY24'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'MAY24'!$D$2:$D$9</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'MAY24'!$E$2:$E$9</f>
+            </numRef>
+          </val>
+        </ser>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -439,12 +1531,12 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,6 +1560,16 @@
           <t>Amount</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Expense Category</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -483,6 +1585,14 @@
       <c r="C2" t="n">
         <v>18</v>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>422.95</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -498,6 +1608,14 @@
       <c r="C3" t="n">
         <v>230</v>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Dining</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>385.17</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -513,11 +1631,19 @@
       <c r="C4" t="n">
         <v>100</v>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1023</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CVS</t>
+          <t>Cvs</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -528,6 +1654,14 @@
       <c r="C5" t="n">
         <v>20</v>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>427</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -543,6 +1677,14 @@
       <c r="C6" t="n">
         <v>20</v>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Misc</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -558,6 +1700,14 @@
       <c r="C7" t="n">
         <v>39</v>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Pet</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>106.83</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -573,6 +1723,14 @@
       <c r="C8" t="n">
         <v>7.7</v>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Shopping</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>139</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -588,6 +1746,14 @@
       <c r="C9" t="n">
         <v>17.62</v>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Snacks</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>150.85</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -682,7 +1848,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>HaagenDaz</t>
+          <t>Haagendaz</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -727,7 +1893,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>McDonald's</t>
+          <t>Mcdonald's</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -847,7 +2013,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>McDonald's</t>
+          <t>Mcdonald's</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -892,7 +2058,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Chick-fil-A</t>
+          <t>Chick-fil-a</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1357,7 +2523,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>McDonald's</t>
+          <t>Mcdonald's</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1399,98 +2565,19 @@
         <v>34</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>Car</t>
-        </is>
-      </c>
-      <c r="B64" t="n">
-        <v>422.95</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>Dining</t>
-        </is>
-      </c>
-      <c r="B65" t="n">
-        <v>385.17</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
-      <c r="B66" t="n">
-        <v>1023</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>Groceries</t>
-        </is>
-      </c>
-      <c r="B67" t="n">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>Misc</t>
-        </is>
-      </c>
-      <c r="B68" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>Pet</t>
-        </is>
-      </c>
-      <c r="B69" t="n">
-        <v>106.83</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>Shopping</t>
-        </is>
-      </c>
-      <c r="B70" t="n">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>Snacks</t>
-        </is>
-      </c>
-      <c r="B71" t="n">
-        <v>150.85</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1514,6 +2601,16 @@
           <t>Amount</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Expense Category</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -1529,6 +2626,14 @@
       <c r="C2" t="n">
         <v>28.27</v>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1544,6 +2649,14 @@
       <c r="C3" t="n">
         <v>43.69</v>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Dining</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>341.81</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1559,6 +2672,14 @@
       <c r="C4" t="n">
         <v>17.72</v>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1574,6 +2695,14 @@
       <c r="C5" t="n">
         <v>109</v>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>221</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1589,6 +2718,14 @@
       <c r="C6" t="n">
         <v>19</v>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Misc</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>406</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1604,6 +2741,14 @@
       <c r="C7" t="n">
         <v>10</v>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Pet</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>125</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1619,6 +2764,14 @@
       <c r="C8" t="n">
         <v>72</v>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Shopping</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>357</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1634,6 +2787,14 @@
       <c r="C9" t="n">
         <v>22</v>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Snacks</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>91</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1653,7 +2814,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Chick-fil-A</t>
+          <t>Chick-fil-a</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1818,7 +2979,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>LAZ Parking</t>
+          <t>Laz Parking</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1908,7 +3069,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Chick-fil-A</t>
+          <t>Chick-fil-a</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2118,7 +3279,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Noah's NY Bagels</t>
+          <t>Noah's Ny Bagels</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2265,98 +3426,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>Car</t>
-        </is>
-      </c>
-      <c r="B52" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>Dining</t>
-        </is>
-      </c>
-      <c r="B53" t="n">
-        <v>341.81</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
-      <c r="B54" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>Groceries</t>
-        </is>
-      </c>
-      <c r="B55" t="n">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>Misc</t>
-        </is>
-      </c>
-      <c r="B56" t="n">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>Pet</t>
-        </is>
-      </c>
-      <c r="B57" t="n">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>Shopping</t>
-        </is>
-      </c>
-      <c r="B58" t="n">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>Snacks</t>
-        </is>
-      </c>
-      <c r="B59" t="n">
-        <v>91</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2380,6 +3462,16 @@
           <t>Amount</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Expense Category</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2395,6 +3487,14 @@
       <c r="C2" t="n">
         <v>200</v>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>335</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -2410,6 +3510,14 @@
       <c r="C3" t="n">
         <v>16</v>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Dining</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>549</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -2425,6 +3533,14 @@
       <c r="C4" t="n">
         <v>10</v>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>761</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -2440,6 +3556,14 @@
       <c r="C5" t="n">
         <v>60</v>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>700</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -2455,6 +3579,14 @@
       <c r="C6" t="n">
         <v>40</v>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Misc</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>110</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -2470,6 +3602,14 @@
       <c r="C7" t="n">
         <v>32</v>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Pet</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>390</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -2485,6 +3625,14 @@
       <c r="C8" t="n">
         <v>16</v>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Shopping</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>2004</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2500,6 +3648,14 @@
       <c r="C9" t="n">
         <v>19</v>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Snacks</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>63</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2849,7 +4005,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>SABAI</t>
+          <t>Sabai</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2894,7 +4050,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>VCA</t>
+          <t>Vca</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -2924,7 +4080,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>VCA</t>
+          <t>Vca</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3014,7 +4170,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>McDonald's</t>
+          <t>Mcdonald's</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3134,7 +4290,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>LV</t>
+          <t>Lv</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -3314,7 +4470,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>85C</t>
+          <t>85c</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -3416,98 +4572,19 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>Car</t>
-        </is>
-      </c>
-      <c r="B71" t="n">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>Dining</t>
-        </is>
-      </c>
-      <c r="B72" t="n">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
-      <c r="B73" t="n">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>Groceries</t>
-        </is>
-      </c>
-      <c r="B74" t="n">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>Misc</t>
-        </is>
-      </c>
-      <c r="B75" t="n">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>Pet</t>
-        </is>
-      </c>
-      <c r="B76" t="n">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>Shopping</t>
-        </is>
-      </c>
-      <c r="B77" t="n">
-        <v>2004</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>Snacks</t>
-        </is>
-      </c>
-      <c r="B78" t="n">
-        <v>63</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3531,6 +4608,16 @@
           <t>Amount</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Expense Category</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -3546,11 +4633,19 @@
       <c r="C2" t="n">
         <v>203</v>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Dining</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>527.6</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SABAI</t>
+          <t>Sabai</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -3561,6 +4656,14 @@
       <c r="C3" t="n">
         <v>54.99</v>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -3576,6 +4679,14 @@
       <c r="C4" t="n">
         <v>42</v>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>385.42</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -3591,6 +4702,14 @@
       <c r="C5" t="n">
         <v>186</v>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Misc</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -3606,6 +4725,14 @@
       <c r="C6" t="n">
         <v>15</v>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Pet</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>54</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -3621,6 +4748,14 @@
       <c r="C7" t="n">
         <v>12.6</v>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Shopping</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>180.69</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -3636,6 +4771,14 @@
       <c r="C8" t="n">
         <v>4.7</v>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Snacks</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -3670,7 +4813,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>85C</t>
+          <t>85c</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -3805,7 +4948,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>LA Parking</t>
+          <t>La Parking</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -3820,7 +4963,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Chick-fil-A</t>
+          <t>Chick-fil-a</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -3910,7 +5053,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>McDonald's</t>
+          <t>Mcdonald's</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -3967,88 +5110,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Dining</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>527.6</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Groceries</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>385.42</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Misc</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Pet</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Shopping</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>180.69</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Snacks</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4072,6 +5146,16 @@
           <t>Amount</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Expense Category</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -4101,16 +5185,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4134,6 +5219,16 @@
           <t>Amount</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Expense Category</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -4149,6 +5244,14 @@
       <c r="C2" t="n">
         <v>152.77</v>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>215.19</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -4164,11 +5267,19 @@
       <c r="C3" t="n">
         <v>86.42</v>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Dining</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>400.77</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>EcoCar</t>
+          <t>Ecocar</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -4179,11 +5290,19 @@
       <c r="C4" t="n">
         <v>16</v>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>215.52</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CVS</t>
+          <t>Cvs</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -4194,6 +5313,14 @@
       <c r="C5" t="n">
         <v>21.79</v>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>384.2</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -4209,6 +5336,14 @@
       <c r="C6" t="n">
         <v>124</v>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Misc</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>222</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -4224,6 +5359,14 @@
       <c r="C7" t="n">
         <v>25</v>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Pet</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>73.2</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -4239,6 +5382,14 @@
       <c r="C8" t="n">
         <v>32.04</v>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Shopping</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>534.48</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -4254,11 +5405,19 @@
       <c r="C9" t="n">
         <v>7.88</v>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Snacks</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>26.41</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>5Below</t>
+          <t>5below</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -4288,7 +5447,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>WestsideDB</t>
+          <t>Westsidedb</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -4333,7 +5492,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>TacoBell</t>
+          <t>Tacobell</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -4453,7 +5612,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CVS</t>
+          <t>Cvs</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -4498,7 +5657,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>SP+</t>
+          <t>Sp+</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -4573,7 +5732,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>LA Eats</t>
+          <t>La Eats</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -4723,7 +5882,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>VCA</t>
+          <t>Vca</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -4993,7 +6152,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>KBBQ</t>
+          <t>Kbbq</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -5020,98 +6179,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>Car</t>
-        </is>
-      </c>
-      <c r="B61" t="n">
-        <v>215.19</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>Dining</t>
-        </is>
-      </c>
-      <c r="B62" t="n">
-        <v>400.77</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
-      <c r="B63" t="n">
-        <v>215.52</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>Groceries</t>
-        </is>
-      </c>
-      <c r="B64" t="n">
-        <v>384.2</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>Misc</t>
-        </is>
-      </c>
-      <c r="B65" t="n">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>Pet</t>
-        </is>
-      </c>
-      <c r="B66" t="n">
-        <v>73.2</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>Shopping</t>
-        </is>
-      </c>
-      <c r="B67" t="n">
-        <v>534.48</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>Snacks</t>
-        </is>
-      </c>
-      <c r="B68" t="n">
-        <v>26.41</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5135,6 +6215,16 @@
           <t>Amount</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Expense Category</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -5150,6 +6240,14 @@
       <c r="C2" t="n">
         <v>120</v>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>263.17</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -5165,6 +6263,14 @@
       <c r="C3" t="n">
         <v>71</v>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Dining</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>781.49</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -5180,6 +6286,14 @@
       <c r="C4" t="n">
         <v>16.39</v>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>98.17</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -5195,6 +6309,14 @@
       <c r="C5" t="n">
         <v>10.56</v>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>665.12</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -5210,6 +6332,14 @@
       <c r="C6" t="n">
         <v>18.99</v>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Misc</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>996.5</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -5225,6 +6355,14 @@
       <c r="C7" t="n">
         <v>5</v>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Pet</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>362.17</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -5240,6 +6378,14 @@
       <c r="C8" t="n">
         <v>18</v>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Shopping</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>950.95</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -5319,7 +6465,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>McDonalds</t>
+          <t>Mcdonalds</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -5349,7 +6495,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>US Post</t>
+          <t>Us Post</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -5364,7 +6510,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>7Eleven</t>
+          <t>7eleven</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -5394,7 +6540,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>McDonalds</t>
+          <t>Mcdonalds</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -5499,7 +6645,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>MCdonalds</t>
+          <t>Mcdonalds</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -5844,7 +6990,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>ARCO</t>
+          <t>Arco</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -6129,7 +7275,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>WinDow</t>
+          <t>Window</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -6144,7 +7290,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>KFC</t>
+          <t>Kfc</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -6174,7 +7320,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>McBoba</t>
+          <t>Mcboba</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -6201,88 +7347,19 @@
         <v>230</v>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>Car</t>
-        </is>
-      </c>
-      <c r="B73" t="n">
-        <v>263.17</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>Dining</t>
-        </is>
-      </c>
-      <c r="B74" t="n">
-        <v>781.49</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
-      <c r="B75" t="n">
-        <v>98.17</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>Groceries</t>
-        </is>
-      </c>
-      <c r="B76" t="n">
-        <v>665.12</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>Misc</t>
-        </is>
-      </c>
-      <c r="B77" t="n">
-        <v>996.5</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>Pet</t>
-        </is>
-      </c>
-      <c r="B78" t="n">
-        <v>362.17</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>Shopping</t>
-        </is>
-      </c>
-      <c r="B79" t="n">
-        <v>950.95</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6306,11 +7383,21 @@
           <t>Amount</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Expense Category</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>McBoba</t>
+          <t>Mcboba</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -6321,6 +7408,14 @@
       <c r="C2" t="n">
         <v>6.75</v>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>123.69</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -6336,6 +7431,14 @@
       <c r="C3" t="n">
         <v>10</v>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Dining</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>208.83</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -6351,6 +7454,14 @@
       <c r="C4" t="n">
         <v>68</v>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>111.29</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -6366,6 +7477,14 @@
       <c r="C5" t="n">
         <v>46</v>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>295.66</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -6381,6 +7500,14 @@
       <c r="C6" t="n">
         <v>9.970000000000001</v>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Misc</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>403.8</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -6396,6 +7523,14 @@
       <c r="C7" t="n">
         <v>12</v>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Pet</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>46</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -6411,6 +7546,14 @@
       <c r="C8" t="n">
         <v>64.55</v>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Shopping</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>196.3</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -6550,7 +7693,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>C2C</t>
+          <t>C2c</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -6565,7 +7708,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>AirB&amp;B</t>
+          <t>Airb&amp;b</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -6670,7 +7813,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>QT</t>
+          <t>Qt</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -6817,88 +7960,19 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Car</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>123.69</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Dining</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>208.83</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>111.29</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>Groceries</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>295.66</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Misc</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>403.8</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>Pet</t>
-        </is>
-      </c>
-      <c r="B41" t="n">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>Shopping</t>
-        </is>
-      </c>
-      <c r="B42" t="n">
-        <v>196.3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6922,6 +7996,16 @@
           <t>Amount</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Expense Category</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -6938,16 +8022,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6971,11 +8056,21 @@
           <t>Amount</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Expense Category</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>QT</t>
+          <t>Qt</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -6986,6 +8081,14 @@
       <c r="C2" t="n">
         <v>8.44</v>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>240.44</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -7001,6 +8104,14 @@
       <c r="C3" t="n">
         <v>50.59</v>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Dining</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>367.59</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -7016,6 +8127,14 @@
       <c r="C4" t="n">
         <v>5.5</v>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>296.99</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -7031,6 +8150,14 @@
       <c r="C5" t="n">
         <v>203.25</v>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>770.54</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -7046,6 +8173,14 @@
       <c r="C6" t="n">
         <v>88.15000000000001</v>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Misc</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>87</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -7061,6 +8196,14 @@
       <c r="C7" t="n">
         <v>40</v>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Pet</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>319</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -7076,6 +8219,14 @@
       <c r="C8" t="n">
         <v>10</v>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Shopping</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>786.79</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -7091,6 +8242,14 @@
       <c r="C9" t="n">
         <v>27</v>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Snacks</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>164.46</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -7335,7 +8494,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>PetSmart</t>
+          <t>Petsmart</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -7410,7 +8569,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>McBoba</t>
+          <t>Mcboba</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -7917,98 +9076,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>Car</t>
-        </is>
-      </c>
-      <c r="B65" t="n">
-        <v>240.44</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>Dining</t>
-        </is>
-      </c>
-      <c r="B66" t="n">
-        <v>367.59</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
-      <c r="B67" t="n">
-        <v>296.99</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>Groceries</t>
-        </is>
-      </c>
-      <c r="B68" t="n">
-        <v>770.54</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>Misc</t>
-        </is>
-      </c>
-      <c r="B69" t="n">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>Pet</t>
-        </is>
-      </c>
-      <c r="B70" t="n">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>Shopping</t>
-        </is>
-      </c>
-      <c r="B71" t="n">
-        <v>786.79</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>Snacks</t>
-        </is>
-      </c>
-      <c r="B72" t="n">
-        <v>164.46</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8032,11 +9112,21 @@
           <t>Amount</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Expense Category</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PetSmart</t>
+          <t>Petsmart</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -8047,6 +9137,14 @@
       <c r="C2" t="n">
         <v>26</v>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -8062,6 +9160,14 @@
       <c r="C3" t="n">
         <v>18</v>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Dining</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>656.54</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -8077,6 +9183,14 @@
       <c r="C4" t="n">
         <v>2.81</v>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>494</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -8092,6 +9206,14 @@
       <c r="C5" t="n">
         <v>45</v>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>660.15</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -8107,11 +9229,19 @@
       <c r="C6" t="n">
         <v>96</v>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Misc</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>162.83</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">McDonald </t>
+          <t xml:space="preserve">Mcdonald </t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -8122,6 +9252,14 @@
       <c r="C7" t="n">
         <v>32</v>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Pet</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>82</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -8137,6 +9275,14 @@
       <c r="C8" t="n">
         <v>13.4</v>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Shopping</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>182</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -8152,6 +9298,14 @@
       <c r="C9" t="n">
         <v>37</v>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Snacks</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>180.83</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -8711,7 +9865,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>QT</t>
+          <t>Qt</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -8876,7 +10030,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t xml:space="preserve">Chick-fil-A </t>
+          <t xml:space="preserve">Chick-fil-a </t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -8951,7 +10105,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>CVS</t>
+          <t>Cvs</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -9098,98 +10252,19 @@
         <v>14</v>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>Car</t>
-        </is>
-      </c>
-      <c r="B73" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>Dining</t>
-        </is>
-      </c>
-      <c r="B74" t="n">
-        <v>656.54</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
-      <c r="B75" t="n">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>Groceries</t>
-        </is>
-      </c>
-      <c r="B76" t="n">
-        <v>660.15</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>Misc</t>
-        </is>
-      </c>
-      <c r="B77" t="n">
-        <v>162.83</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>Pet</t>
-        </is>
-      </c>
-      <c r="B78" t="n">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>Shopping</t>
-        </is>
-      </c>
-      <c r="B79" t="n">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>Snacks</t>
-        </is>
-      </c>
-      <c r="B80" t="n">
-        <v>180.83</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9213,6 +10288,16 @@
           <t>Amount</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Expense Category</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -9228,6 +10313,14 @@
       <c r="C2" t="n">
         <v>31</v>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>110</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -9243,6 +10336,14 @@
       <c r="C3" t="n">
         <v>202</v>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Dining</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>324</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -9258,6 +10359,14 @@
       <c r="C4" t="n">
         <v>5.2</v>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>326</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -9273,6 +10382,14 @@
       <c r="C5" t="n">
         <v>13.45</v>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>876.6900000000001</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -9288,6 +10405,14 @@
       <c r="C6" t="n">
         <v>2.34</v>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Misc</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>265</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -9303,6 +10428,14 @@
       <c r="C7" t="n">
         <v>37</v>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Pet</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -9318,6 +10451,14 @@
       <c r="C8" t="n">
         <v>6</v>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Shopping</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>775.2</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -9333,6 +10474,14 @@
       <c r="C9" t="n">
         <v>25</v>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Snacks</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>131.45</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -9532,7 +10681,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>AMC</t>
+          <t>Amc</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -9592,7 +10741,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>McDonald's</t>
+          <t>Mcdonald's</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -9652,7 +10801,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>AMC</t>
+          <t>Amc</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -9892,7 +11041,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>McDonald's</t>
+          <t>Mcdonald's</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -9952,7 +11101,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>DC Collective</t>
+          <t>Dc Collective</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -10054,98 +11203,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>Car</t>
-        </is>
-      </c>
-      <c r="B58" t="n">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>Dining</t>
-        </is>
-      </c>
-      <c r="B59" t="n">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
-      <c r="B60" t="n">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>Groceries</t>
-        </is>
-      </c>
-      <c r="B61" t="n">
-        <v>876.6900000000001</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>Misc</t>
-        </is>
-      </c>
-      <c r="B62" t="n">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>Pet</t>
-        </is>
-      </c>
-      <c r="B63" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>Shopping</t>
-        </is>
-      </c>
-      <c r="B64" t="n">
-        <v>775.2</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>Snacks</t>
-        </is>
-      </c>
-      <c r="B65" t="n">
-        <v>131.45</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10169,6 +11239,16 @@
           <t>Amount</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Expense Category</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -10184,6 +11264,14 @@
       <c r="C2" t="n">
         <v>28</v>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -10199,6 +11287,14 @@
       <c r="C3" t="n">
         <v>57</v>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Dining</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>318</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -10214,6 +11310,14 @@
       <c r="C4" t="n">
         <v>30</v>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>297</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -10229,6 +11333,14 @@
       <c r="C5" t="n">
         <v>12</v>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>792.9300000000001</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -10244,6 +11356,14 @@
       <c r="C6" t="n">
         <v>5</v>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Misc</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>245</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -10259,6 +11379,14 @@
       <c r="C7" t="n">
         <v>17</v>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Pet</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>218</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -10274,6 +11402,14 @@
       <c r="C8" t="n">
         <v>2</v>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Shopping</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>672</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -10289,6 +11425,14 @@
       <c r="C9" t="n">
         <v>40</v>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Snacks</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>151.75</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -10473,7 +11617,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>85C</t>
+          <t>85c</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -10653,7 +11797,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>TikTok Shop</t>
+          <t>Tiktok Shop</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -10953,7 +12097,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>VCA</t>
+          <t>Vca</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -11070,87 +12214,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>Car</t>
-        </is>
-      </c>
-      <c r="B62" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>Dining</t>
-        </is>
-      </c>
-      <c r="B63" t="n">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>Event</t>
-        </is>
-      </c>
-      <c r="B64" t="n">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>Groceries</t>
-        </is>
-      </c>
-      <c r="B65" t="n">
-        <v>792.9300000000001</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>Misc</t>
-        </is>
-      </c>
-      <c r="B66" t="n">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>Pet</t>
-        </is>
-      </c>
-      <c r="B67" t="n">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>Shopping</t>
-        </is>
-      </c>
-      <c r="B68" t="n">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>Snacks</t>
-        </is>
-      </c>
-      <c r="B69" t="n">
-        <v>151.75</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
created new dataset of all expense data cols (expenditure, category, amount, month/year) to import into tableau
</commit_message>
<xml_diff>
--- a/Expense_Summary.xlsx
+++ b/Expense_Summary.xlsx
@@ -149,7 +149,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>SEP23 Total Expenditure by Category</a:t>
+              <a:t>Yearly Expenses by Category</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -163,7 +163,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'SEP23'!E1</f>
+              <f>'Summary'!B1</f>
             </strRef>
           </tx>
           <spPr>
@@ -173,12 +173,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'SEP23'!$D$2:$D$9</f>
+              <f>'Summary'!$A$2:$A$9</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'SEP23'!$E$2:$E$9</f>
+              <f>'Summary'!$B$2:$B$9</f>
             </numRef>
           </val>
         </ser>
@@ -206,7 +206,64 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>JUN24 Total Expenditure by Category</a:t>
+              <a:t>MAY24 Expenses by Category</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'MAY24'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'MAY24'!$D$2:$D$9</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'MAY24'!$E$2:$E$9</f>
+            </numRef>
+          </val>
+        </ser>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>JUN24 Expenses by Category</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -251,7 +308,7 @@
 </chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
@@ -263,7 +320,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>JUL24 Total Expenditure by Category</a:t>
+              <a:t>JUL24 Expenses by Category</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -308,7 +365,7 @@
 </chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
@@ -320,7 +377,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>AUG24 Total Expenditure by Category</a:t>
+              <a:t>AUG24 Expenses by Category</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -365,7 +422,7 @@
 </chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
@@ -377,7 +434,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>TEMPLATE Total Expenditure by Category</a:t>
+              <a:t>TEMPLATE Expenses by Category</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -434,7 +491,64 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>OCT23 Total Expenditure by Category</a:t>
+              <a:t>SEP23 Expenses by Category</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'SEP23'!E1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'SEP23'!$D$2:$D$9</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'SEP23'!$E$2:$E$9</f>
+            </numRef>
+          </val>
+        </ser>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>OCT23 Expenses by Category</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -479,7 +593,7 @@
 </chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
@@ -491,7 +605,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>NOV23 Total Expenditure by Category</a:t>
+              <a:t>NOV23 Expenses by Category</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -536,7 +650,7 @@
 </chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
@@ -548,7 +662,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>DEC23 Total Expenditure by Category</a:t>
+              <a:t>DEC23 Expenses by Category</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -593,7 +707,7 @@
 </chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
@@ -605,7 +719,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>JAN24 Total Expenditure by Category</a:t>
+              <a:t>JAN24 Expenses by Category</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -650,7 +764,7 @@
 </chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
@@ -662,7 +776,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>FEB24 Total Expenditure by Category</a:t>
+              <a:t>FEB24 Expenses by Category</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -707,7 +821,7 @@
 </chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
@@ -719,7 +833,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>MAR24 Total Expenditure by Category</a:t>
+              <a:t>MAR24 Expenses by Category</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -764,7 +878,7 @@
 </chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
@@ -776,7 +890,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:t>APR24 Total Expenditure by Category</a:t>
+              <a:t>APR24 Expenses by Category</a:t>
             </a:r>
           </a:p>
         </rich>
@@ -806,63 +920,6 @@
           <val>
             <numRef>
               <f>'APR24'!$E$2:$E$9</f>
-            </numRef>
-          </val>
-        </ser>
-        <firstSliceAng val="0"/>
-      </pieChart>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>MAY24 Total Expenditure by Category</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <pieChart>
-        <varyColors val="1"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'MAY24'!E1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'MAY24'!$D$2:$D$9</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'MAY24'!$E$2:$E$9</f>
             </numRef>
           </val>
         </ser>
@@ -987,6 +1044,33 @@
 </file>
 
 <file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -1513,20 +1597,114 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Expense Category</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Car</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1779.44</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Dining</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4860.8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3652.97</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>6178.71</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Misc</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>2953.13</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Pet</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1836.2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Shopping</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>6778.41</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Snacks</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>977.75</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>